<commit_message>
Got rid of older data
</commit_message>
<xml_diff>
--- a/onethirtyseven/static/onethirtyseven/theater_data_csv.xlsx
+++ b/onethirtyseven/static/onethirtyseven/theater_data_csv.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="17080" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,6 +100,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -129,8 +132,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,9 +466,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y29"/>
+  <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:Y27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -585,41 +591,41 @@
       <c r="M2">
         <v>31771.57</v>
       </c>
-      <c r="N2">
-        <v>-0.06</v>
-      </c>
-      <c r="O2">
-        <v>-0.06</v>
-      </c>
-      <c r="P2">
-        <v>0.02</v>
-      </c>
-      <c r="Q2">
+      <c r="N2" s="1">
+        <v>-6.3289999999999999E-2</v>
+      </c>
+      <c r="O2" s="1">
+        <v>-6.2129999999999998E-2</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1.601E-2</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>-1.23E-3</v>
+      </c>
+      <c r="R2" s="1">
+        <v>-1.8010000000000002E-2</v>
+      </c>
+      <c r="S2" s="1">
+        <v>-7.8060000000000004E-2</v>
+      </c>
+      <c r="T2" s="1">
+        <v>-7.6910000000000006E-2</v>
+      </c>
+      <c r="U2" s="1">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>-0.02</v>
-      </c>
-      <c r="S2">
-        <v>-0.08</v>
-      </c>
-      <c r="T2">
-        <v>-0.08</v>
-      </c>
-      <c r="U2">
+      <c r="V2" s="1">
         <v>0</v>
       </c>
-      <c r="V2">
+      <c r="W2" s="1">
         <v>0</v>
       </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>-0.06</v>
-      </c>
-      <c r="Y2">
-        <v>-0.06</v>
+      <c r="X2" s="1">
+        <v>-6.3289999999999999E-2</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>-6.2129999999999998E-2</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -662,41 +668,41 @@
       <c r="M3">
         <v>33876.25</v>
       </c>
-      <c r="N3">
-        <v>0.01</v>
-      </c>
-      <c r="O3">
-        <v>-0.01</v>
-      </c>
-      <c r="P3">
-        <v>0.03</v>
-      </c>
-      <c r="Q3">
-        <v>0.02</v>
-      </c>
-      <c r="R3">
-        <v>0.01</v>
-      </c>
-      <c r="S3">
-        <v>-0.02</v>
-      </c>
-      <c r="T3">
-        <v>-0.04</v>
-      </c>
-      <c r="U3">
+      <c r="N3" s="1">
+        <v>7.9500000000000005E-3</v>
+      </c>
+      <c r="O3" s="1">
+        <v>-1.315E-2</v>
+      </c>
+      <c r="P3" s="1">
+        <v>3.3079999999999998E-2</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>2.1360000000000001E-2</v>
+      </c>
+      <c r="R3" s="1">
+        <v>6.6100000000000004E-3</v>
+      </c>
+      <c r="S3" s="1">
+        <v>-2.4320000000000001E-2</v>
+      </c>
+      <c r="T3" s="1">
+        <v>-4.4749999999999998E-2</v>
+      </c>
+      <c r="U3" s="1">
         <v>0</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="1">
         <v>0</v>
       </c>
-      <c r="W3">
+      <c r="W3" s="1">
         <v>0</v>
       </c>
-      <c r="X3">
-        <v>0.01</v>
-      </c>
-      <c r="Y3">
-        <v>-0.01</v>
+      <c r="X3" s="1">
+        <v>7.9500000000000005E-3</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>-1.315E-2</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -739,41 +745,41 @@
       <c r="M4">
         <v>34327.57</v>
       </c>
-      <c r="N4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="O4">
-        <v>0.06</v>
-      </c>
-      <c r="P4">
-        <v>0.1</v>
-      </c>
-      <c r="Q4">
+      <c r="N4" s="1">
+        <v>6.5170000000000006E-2</v>
+      </c>
+      <c r="O4" s="1">
+        <v>6.1179999999999998E-2</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0.10465000000000001</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>3.7799999999999999E-3</v>
+      </c>
+      <c r="R4" s="1">
+        <v>-1.6570000000000001E-2</v>
+      </c>
+      <c r="S4" s="1">
+        <v>-3.5740000000000001E-2</v>
+      </c>
+      <c r="T4" s="1">
+        <v>-3.9350000000000003E-2</v>
+      </c>
+      <c r="U4" s="1">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="V4" s="1">
         <v>0</v>
       </c>
-      <c r="R4">
-        <v>-0.02</v>
-      </c>
-      <c r="S4">
-        <v>-0.04</v>
-      </c>
-      <c r="T4">
-        <v>-0.04</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0.06</v>
-      </c>
-      <c r="Y4">
-        <v>0.06</v>
+      <c r="W4" s="1">
+        <v>2.0699999999999998E-3</v>
+      </c>
+      <c r="X4" s="1">
+        <v>6.2969999999999998E-2</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>5.8990000000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -816,41 +822,41 @@
       <c r="M5">
         <v>32415.360000000001</v>
       </c>
-      <c r="N5">
-        <v>-0.04</v>
-      </c>
-      <c r="O5">
-        <v>-0.04</v>
-      </c>
-      <c r="P5">
-        <v>0.12</v>
-      </c>
-      <c r="Q5">
-        <v>0.01</v>
-      </c>
-      <c r="R5">
-        <v>-0.03</v>
-      </c>
-      <c r="S5">
-        <v>-0.14000000000000001</v>
-      </c>
-      <c r="T5">
-        <v>-0.15</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>-0.02</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
-        <v>-0.04</v>
-      </c>
-      <c r="Y5">
-        <v>-0.04</v>
+      <c r="N5" s="1">
+        <v>-3.7039999999999997E-2</v>
+      </c>
+      <c r="O5" s="1">
+        <v>-4.1889999999999997E-2</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0.12313</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>5.0699999999999999E-3</v>
+      </c>
+      <c r="R5" s="1">
+        <v>-2.5680000000000001E-2</v>
+      </c>
+      <c r="S5" s="1">
+        <v>-0.14260999999999999</v>
+      </c>
+      <c r="T5" s="1">
+        <v>-0.14693999999999999</v>
+      </c>
+      <c r="U5" s="1">
+        <v>1.8500000000000001E-3</v>
+      </c>
+      <c r="V5" s="1">
+        <v>-1.942E-2</v>
+      </c>
+      <c r="W5" s="1">
+        <v>1.5200000000000001E-3</v>
+      </c>
+      <c r="X5" s="1">
+        <v>-3.85E-2</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>-4.335E-2</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -893,41 +899,41 @@
       <c r="M6">
         <v>33884.11</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>-0.05</v>
-      </c>
-      <c r="P6">
-        <v>0.03</v>
-      </c>
-      <c r="Q6">
-        <v>0.05</v>
-      </c>
-      <c r="R6">
-        <v>0.04</v>
-      </c>
-      <c r="S6">
-        <v>-0.03</v>
-      </c>
-      <c r="T6">
-        <v>-0.08</v>
-      </c>
-      <c r="U6">
-        <v>0.01</v>
-      </c>
-      <c r="V6">
-        <v>-0.02</v>
-      </c>
-      <c r="W6">
-        <v>0.01</v>
-      </c>
-      <c r="X6">
-        <v>-0.01</v>
-      </c>
-      <c r="Y6">
-        <v>-0.06</v>
+      <c r="N6" s="1">
+        <v>-2.82E-3</v>
+      </c>
+      <c r="O6" s="1">
+        <v>-5.21E-2</v>
+      </c>
+      <c r="P6" s="1">
+        <v>2.879E-2</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="R6" s="1">
+        <v>3.5020000000000003E-2</v>
+      </c>
+      <c r="S6" s="1">
+        <v>-3.073E-2</v>
+      </c>
+      <c r="T6" s="1">
+        <v>-7.8630000000000005E-2</v>
+      </c>
+      <c r="U6" s="1">
+        <v>7.6899999999999998E-3</v>
+      </c>
+      <c r="V6" s="1">
+        <v>-1.592E-2</v>
+      </c>
+      <c r="W6" s="1">
+        <v>7.3200000000000001E-3</v>
+      </c>
+      <c r="X6" s="1">
+        <v>-1.0059999999999999E-2</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>-5.8979999999999998E-2</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -970,41 +976,41 @@
       <c r="M7">
         <v>36007.949999999997</v>
       </c>
-      <c r="N7">
-        <v>0.1</v>
-      </c>
-      <c r="O7">
-        <v>0.05</v>
-      </c>
-      <c r="P7">
-        <v>-0.14000000000000001</v>
-      </c>
-      <c r="Q7">
-        <v>0.04</v>
-      </c>
-      <c r="R7">
-        <v>0.05</v>
-      </c>
-      <c r="S7">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="T7">
-        <v>0.23</v>
-      </c>
-      <c r="U7">
-        <v>0.01</v>
-      </c>
-      <c r="V7">
-        <v>-0.01</v>
-      </c>
-      <c r="W7">
-        <v>0.01</v>
-      </c>
-      <c r="X7">
-        <v>0.09</v>
-      </c>
-      <c r="Y7">
-        <v>0.04</v>
+      <c r="N7" s="1">
+        <v>0.10018000000000001</v>
+      </c>
+      <c r="O7" s="1">
+        <v>5.323E-2</v>
+      </c>
+      <c r="P7" s="1">
+        <v>-0.14308999999999999</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>4.4569999999999999E-2</v>
+      </c>
+      <c r="R7" s="1">
+        <v>4.8300000000000003E-2</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0.28388999999999998</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0.22911000000000001</v>
+      </c>
+      <c r="U7" s="1">
+        <v>1.0580000000000001E-2</v>
+      </c>
+      <c r="V7" s="1">
+        <v>-7.9000000000000008E-3</v>
+      </c>
+      <c r="W7" s="1">
+        <v>1.027E-2</v>
+      </c>
+      <c r="X7" s="1">
+        <v>8.899E-2</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>4.2520000000000002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1047,41 +1053,41 @@
       <c r="M8">
         <v>34539.32</v>
       </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>-0.05</v>
-      </c>
-      <c r="P8">
-        <v>-0.04</v>
-      </c>
-      <c r="Q8">
-        <v>0.04</v>
-      </c>
-      <c r="R8">
-        <v>0.01</v>
-      </c>
-      <c r="S8">
-        <v>0.03</v>
-      </c>
-      <c r="T8">
-        <v>-0.01</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8">
-        <v>0</v>
-      </c>
-      <c r="X8">
-        <v>0</v>
-      </c>
-      <c r="Y8">
-        <v>-0.05</v>
+      <c r="N8" s="1">
+        <v>-3.4299999999999999E-3</v>
+      </c>
+      <c r="O8" s="1">
+        <v>-4.5069999999999999E-2</v>
+      </c>
+      <c r="P8" s="1">
+        <v>-3.6450000000000003E-2</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>4.36E-2</v>
+      </c>
+      <c r="R8" s="1">
+        <v>5.0200000000000002E-3</v>
+      </c>
+      <c r="S8" s="1">
+        <v>3.4270000000000002E-2</v>
+      </c>
+      <c r="T8" s="1">
+        <v>-8.94E-3</v>
+      </c>
+      <c r="U8" s="1">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="V8" s="1">
+        <v>-3.15E-3</v>
+      </c>
+      <c r="W8" s="1">
+        <v>1.0300000000000001E-3</v>
+      </c>
+      <c r="X8" s="1">
+        <v>-4.45E-3</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>-4.6050000000000001E-2</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1124,41 +1130,41 @@
       <c r="M9">
         <v>36206.629999999997</v>
       </c>
-      <c r="N9">
-        <v>0.05</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0.04</v>
-      </c>
-      <c r="Q9">
-        <v>0.05</v>
-      </c>
-      <c r="R9">
-        <v>0.02</v>
-      </c>
-      <c r="S9">
-        <v>0.01</v>
-      </c>
-      <c r="T9">
-        <v>-0.04</v>
-      </c>
-      <c r="U9">
-        <v>0.01</v>
-      </c>
-      <c r="V9">
-        <v>-0.02</v>
-      </c>
-      <c r="W9">
-        <v>0.01</v>
-      </c>
-      <c r="X9">
-        <v>0.04</v>
-      </c>
-      <c r="Y9">
-        <v>-0.01</v>
+      <c r="N9" s="1">
+        <v>4.9329999999999999E-2</v>
+      </c>
+      <c r="O9" s="1">
+        <v>-1E-3</v>
+      </c>
+      <c r="P9" s="1">
+        <v>3.7830000000000003E-2</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>5.0380000000000001E-2</v>
+      </c>
+      <c r="R9" s="1">
+        <v>2.129E-2</v>
+      </c>
+      <c r="S9" s="1">
+        <v>1.108E-2</v>
+      </c>
+      <c r="T9" s="1">
+        <v>-3.7409999999999999E-2</v>
+      </c>
+      <c r="U9" s="1">
+        <v>1.043E-2</v>
+      </c>
+      <c r="V9" s="1">
+        <v>-2.308E-2</v>
+      </c>
+      <c r="W9" s="1">
+        <v>9.8700000000000003E-3</v>
+      </c>
+      <c r="X9" s="1">
+        <v>3.9079999999999997E-2</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>-1.076E-2</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1201,41 +1207,41 @@
       <c r="M10">
         <v>36600.29</v>
       </c>
-      <c r="N10">
-        <v>0.04</v>
-      </c>
-      <c r="O10">
-        <v>0.02</v>
-      </c>
-      <c r="P10">
-        <v>0.11</v>
-      </c>
-      <c r="Q10">
-        <v>0.02</v>
-      </c>
-      <c r="R10">
-        <v>-0.01</v>
-      </c>
-      <c r="S10">
-        <v>-0.06</v>
-      </c>
-      <c r="T10">
-        <v>-0.08</v>
-      </c>
-      <c r="U10">
-        <v>0.02</v>
-      </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-      <c r="W10">
-        <v>0.02</v>
-      </c>
-      <c r="X10">
-        <v>0.02</v>
-      </c>
-      <c r="Y10">
-        <v>0</v>
+      <c r="N10" s="1">
+        <v>4.1739999999999999E-2</v>
+      </c>
+      <c r="O10" s="1">
+        <v>1.9429999999999999E-2</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0.11151999999999999</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>2.1839999999999998E-2</v>
+      </c>
+      <c r="R10" s="1">
+        <v>-1.009E-2</v>
+      </c>
+      <c r="S10" s="1">
+        <v>-6.2780000000000002E-2</v>
+      </c>
+      <c r="T10" s="1">
+        <v>-8.2849999999999993E-2</v>
+      </c>
+      <c r="U10" s="1">
+        <v>1.9570000000000001E-2</v>
+      </c>
+      <c r="V10" s="1">
+        <v>3.0899999999999999E-3</v>
+      </c>
+      <c r="W10" s="1">
+        <v>1.9290000000000002E-2</v>
+      </c>
+      <c r="X10" s="1">
+        <v>2.2020000000000001E-2</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>1.3999999999999999E-4</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1278,41 +1284,41 @@
       <c r="M11">
         <v>36595.199999999997</v>
       </c>
-      <c r="N11">
-        <v>-0.06</v>
-      </c>
-      <c r="O11">
-        <v>-0.09</v>
-      </c>
-      <c r="P11">
-        <v>-0.01</v>
-      </c>
-      <c r="Q11">
-        <v>0.03</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>-0.05</v>
-      </c>
-      <c r="T11">
-        <v>-0.08</v>
-      </c>
-      <c r="U11">
-        <v>0.03</v>
-      </c>
-      <c r="V11">
-        <v>0.01</v>
-      </c>
-      <c r="W11">
-        <v>0.03</v>
-      </c>
-      <c r="X11">
-        <v>-0.09</v>
-      </c>
-      <c r="Y11">
-        <v>-0.12</v>
+      <c r="N11" s="1">
+        <v>-5.7570000000000003E-2</v>
+      </c>
+      <c r="O11" s="1">
+        <v>-8.6919999999999997E-2</v>
+      </c>
+      <c r="P11" s="1">
+        <v>-7.26E-3</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>3.2210000000000003E-2</v>
+      </c>
+      <c r="R11" s="1">
+        <v>-1.6199999999999999E-3</v>
+      </c>
+      <c r="S11" s="1">
+        <v>-5.067E-2</v>
+      </c>
+      <c r="T11" s="1">
+        <v>-8.0250000000000002E-2</v>
+      </c>
+      <c r="U11" s="1">
+        <v>3.4779999999999998E-2</v>
+      </c>
+      <c r="V11" s="1">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="W11" s="1">
+        <v>3.4389999999999997E-2</v>
+      </c>
+      <c r="X11" s="1">
+        <v>-8.8900000000000007E-2</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>-0.11728</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1355,41 +1361,41 @@
       <c r="M12">
         <v>41457.39</v>
       </c>
-      <c r="N12">
-        <v>0.02</v>
-      </c>
-      <c r="O12">
-        <v>-0.01</v>
-      </c>
-      <c r="P12">
-        <v>0.09</v>
-      </c>
-      <c r="Q12">
-        <v>0.03</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>-7.0000000000000007E-2</v>
-      </c>
-      <c r="T12">
-        <v>-0.09</v>
-      </c>
-      <c r="U12">
-        <v>0.02</v>
-      </c>
-      <c r="V12">
-        <v>0.01</v>
-      </c>
-      <c r="W12">
-        <v>0.02</v>
-      </c>
-      <c r="X12">
-        <v>-0.01</v>
-      </c>
-      <c r="Y12">
-        <v>-0.04</v>
+      <c r="N12" s="1">
+        <v>1.524E-2</v>
+      </c>
+      <c r="O12" s="1">
+        <v>-1.423E-2</v>
+      </c>
+      <c r="P12" s="1">
+        <v>8.8929999999999995E-2</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>2.9850000000000002E-2</v>
+      </c>
+      <c r="R12" s="1">
+        <v>2.9199999999999999E-3</v>
+      </c>
+      <c r="S12" s="1">
+        <v>-6.7680000000000004E-2</v>
+      </c>
+      <c r="T12" s="1">
+        <v>-9.4729999999999995E-2</v>
+      </c>
+      <c r="U12" s="1">
+        <v>2.2249999999999999E-2</v>
+      </c>
+      <c r="V12" s="1">
+        <v>9.4599999999999997E-3</v>
+      </c>
+      <c r="W12" s="1">
+        <v>2.2020000000000001E-2</v>
+      </c>
+      <c r="X12" s="1">
+        <v>-6.6299999999999996E-3</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>-3.5470000000000002E-2</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -1432,41 +1438,41 @@
       <c r="M13">
         <v>42981.77</v>
       </c>
-      <c r="N13">
-        <v>0.01</v>
-      </c>
-      <c r="O13">
-        <v>-0.03</v>
-      </c>
-      <c r="P13">
-        <v>0.06</v>
-      </c>
-      <c r="Q13">
-        <v>0.04</v>
-      </c>
-      <c r="R13">
-        <v>0.01</v>
-      </c>
-      <c r="S13">
-        <v>-0.04</v>
-      </c>
-      <c r="T13">
-        <v>-0.08</v>
-      </c>
-      <c r="U13">
-        <v>0</v>
-      </c>
-      <c r="V13">
-        <v>-0.05</v>
-      </c>
-      <c r="W13">
-        <v>0</v>
-      </c>
-      <c r="X13">
-        <v>0.01</v>
-      </c>
-      <c r="Y13">
-        <v>-0.03</v>
+      <c r="N13" s="1">
+        <v>9.2499999999999995E-3</v>
+      </c>
+      <c r="O13" s="1">
+        <v>-2.7539999999999999E-2</v>
+      </c>
+      <c r="P13" s="1">
+        <v>5.6370000000000003E-2</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>3.7870000000000001E-2</v>
+      </c>
+      <c r="R13" s="1">
+        <v>1.485E-2</v>
+      </c>
+      <c r="S13" s="1">
+        <v>-4.4600000000000001E-2</v>
+      </c>
+      <c r="T13" s="1">
+        <v>-7.9430000000000001E-2</v>
+      </c>
+      <c r="U13" s="1">
+        <v>-1.7000000000000001E-4</v>
+      </c>
+      <c r="V13" s="1">
+        <v>-4.8050000000000002E-2</v>
+      </c>
+      <c r="W13" s="1">
+        <v>-1.06E-3</v>
+      </c>
+      <c r="X13" s="1">
+        <v>1.0330000000000001E-2</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>-2.6509999999999999E-2</v>
       </c>
     </row>
     <row r="14" spans="1:25">
@@ -1509,41 +1515,41 @@
       <c r="M14">
         <v>44152.1</v>
       </c>
-      <c r="N14">
-        <v>0.09</v>
-      </c>
-      <c r="O14">
-        <v>0.06</v>
-      </c>
-      <c r="P14">
-        <v>-0.01</v>
-      </c>
-      <c r="Q14">
-        <v>0.03</v>
-      </c>
-      <c r="R14">
-        <v>0.01</v>
-      </c>
-      <c r="S14">
-        <v>0.1</v>
-      </c>
-      <c r="T14">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="U14">
-        <v>0.01</v>
-      </c>
-      <c r="V14">
-        <v>-0.02</v>
-      </c>
-      <c r="W14">
-        <v>0.01</v>
-      </c>
-      <c r="X14">
-        <v>0.08</v>
-      </c>
-      <c r="Y14">
-        <v>0.05</v>
+      <c r="N14" s="1">
+        <v>8.8260000000000005E-2</v>
+      </c>
+      <c r="O14" s="1">
+        <v>5.944E-2</v>
+      </c>
+      <c r="P14" s="1">
+        <v>-6.2199999999999998E-3</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>2.6499999999999999E-2</v>
+      </c>
+      <c r="R14" s="1">
+        <v>1.064E-2</v>
+      </c>
+      <c r="S14" s="1">
+        <v>9.5079999999999998E-2</v>
+      </c>
+      <c r="T14" s="1">
+        <v>6.6070000000000004E-2</v>
+      </c>
+      <c r="U14" s="1">
+        <v>5.7099999999999998E-3</v>
+      </c>
+      <c r="V14" s="1">
+        <v>-2.4889999999999999E-2</v>
+      </c>
+      <c r="W14" s="1">
+        <v>5.13E-3</v>
+      </c>
+      <c r="X14" s="1">
+        <v>8.2710000000000006E-2</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>5.4030000000000002E-2</v>
       </c>
     </row>
     <row r="15" spans="1:25">
@@ -1586,41 +1592,41 @@
       <c r="M15">
         <v>41888.69</v>
       </c>
-      <c r="N15">
-        <v>0.1</v>
-      </c>
-      <c r="O15">
-        <v>0.05</v>
-      </c>
-      <c r="P15">
-        <v>0.01</v>
-      </c>
-      <c r="Q15">
-        <v>0.05</v>
-      </c>
-      <c r="R15">
-        <v>0.02</v>
-      </c>
-      <c r="S15">
-        <v>0.09</v>
-      </c>
-      <c r="T15">
-        <v>0.04</v>
-      </c>
-      <c r="U15">
-        <v>-0.02</v>
-      </c>
-      <c r="V15">
+      <c r="N15" s="1">
+        <v>9.8089999999999997E-2</v>
+      </c>
+      <c r="O15" s="1">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="P15" s="1">
+        <v>8.3700000000000007E-3</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>5.0090000000000003E-2</v>
+      </c>
+      <c r="R15" s="1">
+        <v>2.104E-2</v>
+      </c>
+      <c r="S15" s="1">
+        <v>8.8980000000000004E-2</v>
+      </c>
+      <c r="T15" s="1">
+        <v>3.8120000000000001E-2</v>
+      </c>
+      <c r="U15" s="1">
+        <v>-2.4459999999999999E-2</v>
+      </c>
+      <c r="V15" s="1">
         <v>0</v>
       </c>
-      <c r="W15">
-        <v>-0.02</v>
-      </c>
-      <c r="X15">
-        <v>0.13</v>
-      </c>
-      <c r="Y15">
-        <v>7.0000000000000007E-2</v>
+      <c r="W15" s="1">
+        <v>-2.4E-2</v>
+      </c>
+      <c r="X15" s="1">
+        <v>0.12509000000000001</v>
+      </c>
+      <c r="Y15" s="1">
+        <v>7.2539999999999993E-2</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -1663,41 +1669,41 @@
       <c r="M16">
         <v>39055.5</v>
       </c>
-      <c r="N16">
-        <v>0.03</v>
-      </c>
-      <c r="O16">
-        <v>-0.03</v>
-      </c>
-      <c r="P16">
-        <v>0.04</v>
-      </c>
-      <c r="Q16">
-        <v>0.06</v>
-      </c>
-      <c r="R16">
-        <v>0.03</v>
-      </c>
-      <c r="S16">
-        <v>-0.01</v>
-      </c>
-      <c r="T16">
-        <v>-0.06</v>
-      </c>
-      <c r="U16">
-        <v>-0.02</v>
-      </c>
-      <c r="V16">
+      <c r="N16" s="1">
+        <v>2.86E-2</v>
+      </c>
+      <c r="O16" s="1">
+        <v>-3.0300000000000001E-2</v>
+      </c>
+      <c r="P16" s="1">
+        <v>3.6880000000000003E-2</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>6.1019999999999998E-2</v>
+      </c>
+      <c r="R16" s="1">
+        <v>2.6519999999999998E-2</v>
+      </c>
+      <c r="S16" s="1">
+        <v>-7.9799999999999992E-3</v>
+      </c>
+      <c r="T16" s="1">
+        <v>-6.479E-2</v>
+      </c>
+      <c r="U16" s="1">
+        <v>-2.0629999999999999E-2</v>
+      </c>
+      <c r="V16" s="1">
         <v>0</v>
       </c>
-      <c r="W16">
-        <v>-0.02</v>
-      </c>
-      <c r="X16">
-        <v>0.05</v>
-      </c>
-      <c r="Y16">
-        <v>-0.01</v>
+      <c r="W16" s="1">
+        <v>-2.0250000000000001E-2</v>
+      </c>
+      <c r="X16" s="1">
+        <v>4.9860000000000002E-2</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>-1.026E-2</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -1740,41 +1746,41 @@
       <c r="M17">
         <v>39460.29</v>
       </c>
-      <c r="N17">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="O17">
-        <v>-0.01</v>
-      </c>
-      <c r="P17">
-        <v>-0.09</v>
-      </c>
-      <c r="Q17">
-        <v>0.08</v>
-      </c>
-      <c r="R17">
-        <v>0.06</v>
-      </c>
-      <c r="S17">
-        <v>0.18</v>
-      </c>
-      <c r="T17">
-        <v>0.09</v>
-      </c>
-      <c r="U17">
-        <v>0.09</v>
-      </c>
-      <c r="V17">
-        <v>-0.09</v>
-      </c>
-      <c r="W17">
-        <v>0.09</v>
-      </c>
-      <c r="X17">
-        <v>-0.01</v>
-      </c>
-      <c r="Y17">
-        <v>-0.09</v>
+      <c r="N17" s="1">
+        <v>7.1809999999999999E-2</v>
+      </c>
+      <c r="O17" s="1">
+        <v>-1.047E-2</v>
+      </c>
+      <c r="P17" s="1">
+        <v>-9.4299999999999995E-2</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>8.3159999999999998E-2</v>
+      </c>
+      <c r="R17" s="1">
+        <v>5.9749999999999998E-2</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0.18340999999999999</v>
+      </c>
+      <c r="T17" s="1">
+        <v>9.2560000000000003E-2</v>
+      </c>
+      <c r="U17" s="1">
+        <v>9.0670000000000001E-2</v>
+      </c>
+      <c r="V17" s="1">
+        <v>-8.9330000000000007E-2</v>
+      </c>
+      <c r="W17" s="1">
+        <v>8.6720000000000005E-2</v>
+      </c>
+      <c r="X17" s="1">
+        <v>-1.372E-2</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>-8.9429999999999996E-2</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -1817,41 +1823,41 @@
       <c r="M18">
         <v>43335.87</v>
       </c>
-      <c r="N18">
-        <v>0.09</v>
-      </c>
-      <c r="O18">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0.02</v>
-      </c>
-      <c r="R18">
-        <v>0.01</v>
-      </c>
-      <c r="S18">
-        <v>0.09</v>
-      </c>
-      <c r="T18">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="U18">
-        <v>0.08</v>
-      </c>
-      <c r="V18">
-        <v>-0.08</v>
-      </c>
-      <c r="W18">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="X18">
-        <v>0.02</v>
-      </c>
-      <c r="Y18">
-        <v>0</v>
+      <c r="N18" s="1">
+        <v>9.1600000000000001E-2</v>
+      </c>
+      <c r="O18" s="1">
+        <v>6.7019999999999996E-2</v>
+      </c>
+      <c r="P18" s="1">
+        <v>-1.9599999999999999E-3</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>2.179E-2</v>
+      </c>
+      <c r="R18" s="1">
+        <v>6.11E-3</v>
+      </c>
+      <c r="S18" s="1">
+        <v>9.3740000000000004E-2</v>
+      </c>
+      <c r="T18" s="1">
+        <v>6.9110000000000005E-2</v>
+      </c>
+      <c r="U18" s="1">
+        <v>7.6259999999999994E-2</v>
+      </c>
+      <c r="V18" s="1">
+        <v>-7.9750000000000001E-2</v>
+      </c>
+      <c r="W18" s="1">
+        <v>7.2270000000000001E-2</v>
+      </c>
+      <c r="X18" s="1">
+        <v>1.8020000000000001E-2</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>-4.8999999999999998E-3</v>
       </c>
     </row>
     <row r="19" spans="1:25">
@@ -1894,41 +1900,41 @@
       <c r="M19">
         <v>43549.35</v>
       </c>
-      <c r="N19">
-        <v>0.08</v>
-      </c>
-      <c r="O19">
-        <v>0.04</v>
-      </c>
-      <c r="P19">
-        <v>0.08</v>
-      </c>
-      <c r="Q19">
-        <v>0.04</v>
-      </c>
-      <c r="R19">
-        <v>0.02</v>
-      </c>
-      <c r="S19">
-        <v>-0.01</v>
-      </c>
-      <c r="T19">
-        <v>-0.04</v>
-      </c>
-      <c r="U19">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="V19">
-        <v>-0.01</v>
-      </c>
-      <c r="W19">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="X19">
-        <v>0</v>
-      </c>
-      <c r="Y19">
-        <v>-0.03</v>
+      <c r="N19" s="1">
+        <v>7.6869999999999994E-2</v>
+      </c>
+      <c r="O19" s="1">
+        <v>3.6679999999999997E-2</v>
+      </c>
+      <c r="P19" s="1">
+        <v>8.2799999999999999E-2</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>3.8460000000000001E-2</v>
+      </c>
+      <c r="R19" s="1">
+        <v>1.5169999999999999E-2</v>
+      </c>
+      <c r="S19" s="1">
+        <v>-5.4799999999999996E-3</v>
+      </c>
+      <c r="T19" s="1">
+        <v>-4.2599999999999999E-2</v>
+      </c>
+      <c r="U19" s="1">
+        <v>7.4209999999999998E-2</v>
+      </c>
+      <c r="V19" s="1">
+        <v>-1.332E-2</v>
+      </c>
+      <c r="W19" s="1">
+        <v>7.1779999999999997E-2</v>
+      </c>
+      <c r="X19" s="1">
+        <v>4.7499999999999999E-3</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>-3.2750000000000001E-2</v>
       </c>
     </row>
     <row r="20" spans="1:25">
@@ -1971,41 +1977,41 @@
       <c r="M20">
         <v>45023.71</v>
       </c>
-      <c r="N20">
-        <v>0.08</v>
-      </c>
-      <c r="O20">
-        <v>0.06</v>
-      </c>
-      <c r="P20">
-        <v>0.15</v>
-      </c>
-      <c r="Q20">
-        <v>0.02</v>
-      </c>
-      <c r="R20">
-        <v>-0.01</v>
-      </c>
-      <c r="S20">
-        <v>-0.06</v>
-      </c>
-      <c r="T20">
-        <v>-7.0000000000000007E-2</v>
-      </c>
-      <c r="U20">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="V20">
-        <v>-0.03</v>
-      </c>
-      <c r="W20">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="X20">
-        <v>0.01</v>
-      </c>
-      <c r="Y20">
-        <v>-0.01</v>
+      <c r="N20" s="1">
+        <v>7.6090000000000005E-2</v>
+      </c>
+      <c r="O20" s="1">
+        <v>6.019E-2</v>
+      </c>
+      <c r="P20" s="1">
+        <v>0.14599000000000001</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>1.609E-2</v>
+      </c>
+      <c r="R20" s="1">
+        <v>-1.3050000000000001E-2</v>
+      </c>
+      <c r="S20" s="1">
+        <v>-6.0990000000000003E-2</v>
+      </c>
+      <c r="T20" s="1">
+        <v>-7.4859999999999996E-2</v>
+      </c>
+      <c r="U20" s="1">
+        <v>7.0749999999999993E-2</v>
+      </c>
+      <c r="V20" s="1">
+        <v>-2.5940000000000001E-2</v>
+      </c>
+      <c r="W20" s="1">
+        <v>6.7809999999999995E-2</v>
+      </c>
+      <c r="X20" s="1">
+        <v>7.7600000000000004E-3</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>-7.1300000000000001E-3</v>
       </c>
     </row>
     <row r="21" spans="1:25">
@@ -2048,41 +2054,41 @@
       <c r="M21">
         <v>45347.12</v>
       </c>
-      <c r="N21">
-        <v>0.02</v>
-      </c>
-      <c r="O21">
-        <v>-0.02</v>
-      </c>
-      <c r="P21">
-        <v>-0.09</v>
-      </c>
-      <c r="Q21">
-        <v>0.04</v>
-      </c>
-      <c r="R21">
-        <v>0.01</v>
-      </c>
-      <c r="S21">
-        <v>0.12</v>
-      </c>
-      <c r="T21">
-        <v>0.08</v>
-      </c>
-      <c r="U21">
-        <v>0.05</v>
-      </c>
-      <c r="V21">
-        <v>-0.01</v>
-      </c>
-      <c r="W21">
-        <v>0.04</v>
-      </c>
-      <c r="X21">
-        <v>-0.02</v>
-      </c>
-      <c r="Y21">
-        <v>-0.06</v>
+      <c r="N21" s="1">
+        <v>1.8030000000000001E-2</v>
+      </c>
+      <c r="O21" s="1">
+        <v>-2.2530000000000001E-2</v>
+      </c>
+      <c r="P21" s="1">
+        <v>-9.2719999999999997E-2</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>4.0669999999999998E-2</v>
+      </c>
+      <c r="R21" s="1">
+        <v>1.1990000000000001E-2</v>
+      </c>
+      <c r="S21" s="1">
+        <v>0.12206</v>
+      </c>
+      <c r="T21" s="1">
+        <v>7.7359999999999998E-2</v>
+      </c>
+      <c r="U21" s="1">
+        <v>4.5100000000000001E-2</v>
+      </c>
+      <c r="V21" s="1">
+        <v>-1.281E-2</v>
+      </c>
+      <c r="W21" s="1">
+        <v>4.3240000000000001E-2</v>
+      </c>
+      <c r="X21" s="1">
+        <v>-2.4160000000000001E-2</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>-6.3039999999999999E-2</v>
       </c>
     </row>
     <row r="22" spans="1:25">
@@ -2125,41 +2131,41 @@
       <c r="M22">
         <v>48398.22</v>
       </c>
-      <c r="N22">
-        <v>0.05</v>
-      </c>
-      <c r="O22">
-        <v>0.04</v>
-      </c>
-      <c r="P22">
-        <v>-0.02</v>
-      </c>
-      <c r="Q22">
-        <v>0.01</v>
-      </c>
-      <c r="R22">
-        <v>-0.02</v>
-      </c>
-      <c r="S22">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="T22">
-        <v>0.06</v>
-      </c>
-      <c r="U22">
-        <v>0.04</v>
-      </c>
-      <c r="V22">
-        <v>0.03</v>
-      </c>
-      <c r="W22">
-        <v>0.04</v>
-      </c>
-      <c r="X22">
-        <v>0.01</v>
-      </c>
-      <c r="Y22">
-        <v>0</v>
+      <c r="N22" s="1">
+        <v>4.6949999999999999E-2</v>
+      </c>
+      <c r="O22" s="1">
+        <v>3.8339999999999999E-2</v>
+      </c>
+      <c r="P22" s="1">
+        <v>-1.9480000000000001E-2</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>9.6600000000000002E-3</v>
+      </c>
+      <c r="R22" s="1">
+        <v>-1.555E-2</v>
+      </c>
+      <c r="S22" s="1">
+        <v>6.7750000000000005E-2</v>
+      </c>
+      <c r="T22" s="1">
+        <v>5.8970000000000002E-2</v>
+      </c>
+      <c r="U22" s="1">
+        <v>4.199E-2</v>
+      </c>
+      <c r="V22" s="1">
+        <v>2.6280000000000001E-2</v>
+      </c>
+      <c r="W22" s="1">
+        <v>4.1480000000000003E-2</v>
+      </c>
+      <c r="X22" s="1">
+        <v>5.2500000000000003E-3</v>
+      </c>
+      <c r="Y22" s="1">
+        <v>-3.0100000000000001E-3</v>
       </c>
     </row>
     <row r="23" spans="1:25">
@@ -2202,41 +2208,41 @@
       <c r="M23">
         <v>48544.45</v>
       </c>
-      <c r="N23">
-        <v>0.06</v>
-      </c>
-      <c r="O23">
-        <v>0.06</v>
-      </c>
-      <c r="P23">
-        <v>-0.04</v>
-      </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-      <c r="R23">
-        <v>-0.03</v>
-      </c>
-      <c r="S23">
-        <v>0.1</v>
-      </c>
-      <c r="T23">
-        <v>0.1</v>
-      </c>
-      <c r="U23">
-        <v>0.02</v>
-      </c>
-      <c r="V23">
-        <v>-0.04</v>
-      </c>
-      <c r="W23">
-        <v>0.02</v>
-      </c>
-      <c r="X23">
-        <v>0.04</v>
-      </c>
-      <c r="Y23">
-        <v>0.04</v>
+      <c r="N23" s="1">
+        <v>5.8139999999999997E-2</v>
+      </c>
+      <c r="O23" s="1">
+        <v>6.0350000000000001E-2</v>
+      </c>
+      <c r="P23" s="1">
+        <v>-3.7499999999999999E-2</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>-2.4099999999999998E-3</v>
+      </c>
+      <c r="R23" s="1">
+        <v>-3.141E-2</v>
+      </c>
+      <c r="S23" s="1">
+        <v>9.937E-2</v>
+      </c>
+      <c r="T23" s="1">
+        <v>0.10166</v>
+      </c>
+      <c r="U23" s="1">
+        <v>1.8280000000000001E-2</v>
+      </c>
+      <c r="V23" s="1">
+        <v>-3.7929999999999998E-2</v>
+      </c>
+      <c r="W23" s="1">
+        <v>1.634E-2</v>
+      </c>
+      <c r="X23" s="1">
+        <v>4.113E-2</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>4.3299999999999998E-2</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -2279,41 +2285,41 @@
       <c r="M24">
         <v>46529.71</v>
       </c>
-      <c r="N24">
-        <v>0.01</v>
-      </c>
-      <c r="O24">
-        <v>0.03</v>
-      </c>
-      <c r="P24">
-        <v>0.05</v>
-      </c>
-      <c r="Q24">
-        <v>-0.01</v>
-      </c>
-      <c r="R24">
-        <v>-0.04</v>
-      </c>
-      <c r="S24">
-        <v>-0.03</v>
-      </c>
-      <c r="T24">
-        <v>-0.02</v>
-      </c>
-      <c r="U24">
-        <v>0.03</v>
-      </c>
-      <c r="V24">
-        <v>-0.03</v>
-      </c>
-      <c r="W24">
-        <v>0.02</v>
-      </c>
-      <c r="X24">
-        <v>-0.01</v>
-      </c>
-      <c r="Y24">
-        <v>0.01</v>
+      <c r="N24" s="1">
+        <v>1.4120000000000001E-2</v>
+      </c>
+      <c r="O24" s="1">
+        <v>2.8580000000000001E-2</v>
+      </c>
+      <c r="P24" s="1">
+        <v>4.8030000000000003E-2</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>-1.4250000000000001E-2</v>
+      </c>
+      <c r="R24" s="1">
+        <v>-4.3060000000000001E-2</v>
+      </c>
+      <c r="S24" s="1">
+        <v>-3.236E-2</v>
+      </c>
+      <c r="T24" s="1">
+        <v>-1.856E-2</v>
+      </c>
+      <c r="U24" s="1">
+        <v>2.5440000000000001E-2</v>
+      </c>
+      <c r="V24" s="1">
+        <v>-3.2259999999999997E-2</v>
+      </c>
+      <c r="W24" s="1">
+        <v>2.334E-2</v>
+      </c>
+      <c r="X24" s="1">
+        <v>-9.0100000000000006E-3</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>5.1200000000000004E-3</v>
       </c>
     </row>
     <row r="25" spans="1:25">
@@ -2356,41 +2362,41 @@
       <c r="M25">
         <v>46292.46</v>
       </c>
-      <c r="N25">
-        <v>-0.04</v>
-      </c>
-      <c r="O25">
-        <v>-0.04</v>
-      </c>
-      <c r="P25">
-        <v>0.12</v>
-      </c>
-      <c r="Q25">
-        <v>0</v>
-      </c>
-      <c r="R25">
-        <v>-0.04</v>
-      </c>
-      <c r="S25">
-        <v>-0.14000000000000001</v>
-      </c>
-      <c r="T25">
-        <v>-0.14000000000000001</v>
-      </c>
-      <c r="U25">
-        <v>0.04</v>
-      </c>
-      <c r="V25">
-        <v>-0.01</v>
-      </c>
-      <c r="W25">
-        <v>0.03</v>
-      </c>
-      <c r="X25">
-        <v>-0.08</v>
-      </c>
-      <c r="Y25">
-        <v>-7.0000000000000007E-2</v>
+      <c r="N25" s="1">
+        <v>-4.3529999999999999E-2</v>
+      </c>
+      <c r="O25" s="1">
+        <v>-4.0379999999999999E-2</v>
+      </c>
+      <c r="P25" s="1">
+        <v>0.11706999999999999</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>-4.7299999999999998E-3</v>
+      </c>
+      <c r="R25" s="1">
+        <v>-4.4920000000000002E-2</v>
+      </c>
+      <c r="S25" s="1">
+        <v>-0.14377000000000001</v>
+      </c>
+      <c r="T25" s="1">
+        <v>-0.14094999999999999</v>
+      </c>
+      <c r="U25" s="1">
+        <v>3.6499999999999998E-2</v>
+      </c>
+      <c r="V25" s="1">
+        <v>-1.209E-2</v>
+      </c>
+      <c r="W25" s="1">
+        <v>3.4639999999999997E-2</v>
+      </c>
+      <c r="X25" s="1">
+        <v>-7.5560000000000002E-2</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>-7.2510000000000005E-2</v>
       </c>
     </row>
     <row r="26" spans="1:25">
@@ -2433,41 +2439,41 @@
       <c r="M26">
         <v>49911.82</v>
       </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="O26">
-        <v>-0.06</v>
-      </c>
-      <c r="P26">
-        <v>-0.18</v>
-      </c>
-      <c r="Q26">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="R26">
-        <v>0.01</v>
-      </c>
-      <c r="S26">
-        <v>0.22</v>
-      </c>
-      <c r="T26">
-        <v>0.15</v>
-      </c>
-      <c r="U26">
-        <v>0.05</v>
-      </c>
-      <c r="V26">
-        <v>-0.1</v>
-      </c>
-      <c r="W26">
-        <v>0.04</v>
-      </c>
-      <c r="X26">
-        <v>-0.04</v>
-      </c>
-      <c r="Y26">
-        <v>-0.09</v>
+      <c r="N26" s="1">
+        <v>-2.3E-3</v>
+      </c>
+      <c r="O26" s="1">
+        <v>-5.876E-2</v>
+      </c>
+      <c r="P26" s="1">
+        <v>-0.18326999999999999</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>6.5490000000000007E-2</v>
+      </c>
+      <c r="R26" s="1">
+        <v>1.0869999999999999E-2</v>
+      </c>
+      <c r="S26" s="1">
+        <v>0.22156999999999999</v>
+      </c>
+      <c r="T26" s="1">
+        <v>0.15245</v>
+      </c>
+      <c r="U26" s="1">
+        <v>4.5510000000000002E-2</v>
+      </c>
+      <c r="V26" s="1">
+        <v>-0.10256</v>
+      </c>
+      <c r="W26" s="1">
+        <v>3.8960000000000002E-2</v>
+      </c>
+      <c r="X26" s="1">
+        <v>-3.9719999999999998E-2</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>-9.4049999999999995E-2</v>
       </c>
     </row>
     <row r="27" spans="1:25">
@@ -2510,195 +2516,41 @@
       <c r="M27">
         <v>55093.58</v>
       </c>
-      <c r="N27">
-        <v>0.13</v>
-      </c>
-      <c r="O27">
-        <v>0.16</v>
-      </c>
-      <c r="P27">
-        <v>-0.02</v>
-      </c>
-      <c r="Q27">
-        <v>-0.03</v>
-      </c>
-      <c r="R27">
-        <v>-0.08</v>
-      </c>
-      <c r="S27">
-        <v>0.15</v>
-      </c>
-      <c r="T27">
-        <v>0.18</v>
-      </c>
-      <c r="U27">
-        <v>0.01</v>
-      </c>
-      <c r="V27">
-        <v>-0.32</v>
-      </c>
-      <c r="W27">
-        <v>-0.01</v>
-      </c>
-      <c r="X27">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="Y27">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25">
-      <c r="A28">
-        <v>1988</v>
-      </c>
-      <c r="B28">
-        <v>4458.3999999999996</v>
-      </c>
-      <c r="C28">
-        <v>1084.8</v>
-      </c>
-      <c r="D28">
-        <v>510</v>
-      </c>
-      <c r="E28">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="F28">
-        <v>8.23</v>
-      </c>
-      <c r="G28">
-        <v>8.74</v>
-      </c>
-      <c r="H28">
-        <v>2.13</v>
-      </c>
-      <c r="I28">
-        <v>21632</v>
-      </c>
-      <c r="J28">
-        <v>1497</v>
-      </c>
-      <c r="K28">
-        <v>23129</v>
-      </c>
-      <c r="L28">
-        <v>192762.33</v>
-      </c>
-      <c r="M28">
-        <v>46902.16</v>
-      </c>
-      <c r="N28">
-        <v>0.05</v>
-      </c>
-      <c r="O28">
-        <v>0</v>
-      </c>
-      <c r="P28">
-        <v>0</v>
-      </c>
-      <c r="Q28">
-        <v>0.05</v>
-      </c>
-      <c r="R28">
-        <v>0.01</v>
-      </c>
-      <c r="S28">
-        <v>0.05</v>
-      </c>
-      <c r="T28">
-        <v>-0.01</v>
-      </c>
-      <c r="U28">
-        <v>0.05</v>
-      </c>
-      <c r="V28">
-        <v>-0.28000000000000003</v>
-      </c>
-      <c r="W28">
-        <v>0.02</v>
-      </c>
-      <c r="X28">
-        <v>0.03</v>
-      </c>
-      <c r="Y28">
-        <v>-0.02</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25">
-      <c r="A29">
-        <v>1987</v>
-      </c>
-      <c r="B29">
-        <v>4252.8999999999996</v>
-      </c>
-      <c r="C29">
-        <v>1088.5</v>
-      </c>
-      <c r="D29">
-        <v>509</v>
-      </c>
-      <c r="E29">
-        <v>3.91</v>
-      </c>
-      <c r="F29">
-        <v>8.16</v>
-      </c>
-      <c r="G29">
-        <v>8.36</v>
-      </c>
-      <c r="H29">
-        <v>2.14</v>
-      </c>
-      <c r="I29">
-        <v>20595</v>
-      </c>
-      <c r="J29">
-        <v>2084</v>
-      </c>
-      <c r="K29">
-        <v>22679</v>
-      </c>
-      <c r="L29">
-        <v>187525.91</v>
-      </c>
-      <c r="M29">
-        <v>47995.94</v>
-      </c>
-      <c r="N29">
-        <v>0.13</v>
-      </c>
-      <c r="O29">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="P29">
-        <v>0.13</v>
-      </c>
-      <c r="Q29">
-        <v>0.05</v>
-      </c>
-      <c r="R29">
-        <v>0.02</v>
-      </c>
-      <c r="S29">
-        <v>0</v>
-      </c>
-      <c r="T29">
-        <v>-0.05</v>
-      </c>
-      <c r="U29">
-        <v>0</v>
-      </c>
-      <c r="V29">
-        <v>0</v>
-      </c>
-      <c r="W29">
-        <v>0</v>
-      </c>
-      <c r="X29">
-        <v>0</v>
-      </c>
-      <c r="Y29">
-        <v>0</v>
+      <c r="N27" s="1">
+        <v>0.12897</v>
+      </c>
+      <c r="O27" s="1">
+        <v>0.16409000000000001</v>
+      </c>
+      <c r="P27" s="1">
+        <v>-1.5689999999999999E-2</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>-3.406E-2</v>
+      </c>
+      <c r="R27" s="1">
+        <v>-7.8469999999999998E-2</v>
+      </c>
+      <c r="S27" s="1">
+        <v>0.14696000000000001</v>
+      </c>
+      <c r="T27" s="1">
+        <v>0.18264</v>
+      </c>
+      <c r="U27" s="1">
+        <v>1.2710000000000001E-2</v>
+      </c>
+      <c r="V27" s="1">
+        <v>-0.32264999999999999</v>
+      </c>
+      <c r="W27" s="1">
+        <v>-8.9899999999999997E-3</v>
+      </c>
+      <c r="X27" s="1">
+        <v>0.13922000000000001</v>
+      </c>
+      <c r="Y27" s="1">
+        <v>0.17465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>